<commit_message>
Adding `json` (logical) and `source` (string) to the codebook.
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enzinger\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzprante/GitHub/MORPEP/META CMP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B04AB9-69E4-4BAA-911C-36DA4081ED24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58FBF8B-6395-B441-9C58-DC78FE6E25B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4AE10940-A047-2F4D-80AE-0938BE2B299E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{4AE10940-A047-2F4D-80AE-0938BE2B299E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$1:$J$117</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="233">
   <si>
     <t>Category</t>
   </si>
@@ -673,6 +673,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (add here on the fly)</t>
     </r>
@@ -817,12 +818,39 @@
   <si>
     <t xml:space="preserve">Reason for exclusion after full text screening </t>
   </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>zotero</t>
+  </si>
+  <si>
+    <t>researcher</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>study/own_calculation</t>
+  </si>
+  <si>
+    <t>public_database</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -874,17 +902,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -896,6 +920,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -944,14 +969,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1267,26 +1292,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C77282-C0D9-FE44-835B-2F72376F6C5B}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C76" sqref="C76"/>
+      <selection pane="bottomRight" activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="87.125" customWidth="1"/>
-    <col min="4" max="4" width="11.875" customWidth="1"/>
-    <col min="5" max="5" width="16.25" customWidth="1"/>
-    <col min="6" max="7" width="40.625" customWidth="1"/>
-    <col min="8" max="9" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="87.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="9" width="40.6640625" customWidth="1"/>
+    <col min="10" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1309,16 +1335,22 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1334,13 +1366,19 @@
       <c r="E2" s="1"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+      <c r="H2" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1358,13 +1396,19 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>11</v>
+      <c r="H3" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1382,13 +1426,19 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
-        <v>11</v>
+      <c r="H4" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1404,13 +1454,19 @@
       <c r="E5" s="6"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>11</v>
+      <c r="H5" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1426,13 +1482,19 @@
       <c r="E6" s="1"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>11</v>
+      <c r="H6" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1450,15 +1512,21 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1">
+      <c r="H7" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1476,15 +1544,21 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1">
+      <c r="H8" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1502,15 +1576,21 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="47.25">
+      <c r="H9" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1530,15 +1610,21 @@
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="126">
+      <c r="H10" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1558,15 +1644,21 @@
         <v>27</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="94.5">
+      <c r="H11" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1584,41 +1676,53 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="47.25">
+      <c r="H12" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="1" t="s">
         <v>203</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="H13" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1636,22 +1740,28 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="47.25">
+      <c r="H14" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -1664,15 +1774,21 @@
         <v>35</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="126">
+      <c r="H15" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1694,15 +1810,21 @@
       <c r="G16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" ht="31.5">
+      <c r="H16" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1722,15 +1844,21 @@
         <v>39</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="94.5">
+      <c r="H17" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1752,15 +1880,21 @@
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="31.5">
+      <c r="H18" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1782,15 +1916,21 @@
       <c r="G19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="31.5">
+      <c r="H19" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1812,15 +1952,21 @@
       <c r="G20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="63">
+      <c r="H20" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1842,15 +1988,21 @@
       <c r="G21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" ht="31.5">
+      <c r="H21" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1872,15 +2024,21 @@
       <c r="G22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" ht="31.5">
+      <c r="H22" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1900,15 +2058,21 @@
       <c r="G23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" ht="31.5">
+      <c r="H23" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1928,15 +2092,21 @@
       <c r="G24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" ht="31.5">
+      <c r="H24" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1956,15 +2126,21 @@
         <v>39</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" ht="31.5">
+      <c r="H25" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -1984,15 +2160,21 @@
         <v>39</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5">
+      <c r="H26" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2012,15 +2194,21 @@
         <v>31</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" ht="31.5">
+      <c r="H27" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>68</v>
       </c>
@@ -2040,15 +2228,21 @@
         <v>52</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" ht="31.5">
+      <c r="H28" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -2058,23 +2252,29 @@
       <c r="C29" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="1" t="s">
         <v>217</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" ht="31.5">
+      <c r="H29" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
@@ -2094,15 +2294,21 @@
         <v>78</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="H30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" ht="31.5">
+      <c r="H30" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -2122,15 +2328,21 @@
         <v>78</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" ht="31.5">
+      <c r="H31" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -2148,15 +2360,21 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" ht="31.5">
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>68</v>
       </c>
@@ -2176,15 +2394,21 @@
         <v>78</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" ht="31.5">
+      <c r="H33" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>68</v>
       </c>
@@ -2202,15 +2426,21 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" ht="47.25">
+      <c r="H34" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>88</v>
       </c>
@@ -2230,15 +2460,21 @@
       <c r="G35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" ht="31.5">
+      <c r="H35" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>88</v>
       </c>
@@ -2256,15 +2492,21 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" ht="47.25">
+      <c r="H36" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
@@ -2282,15 +2524,21 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" ht="47.25">
+      <c r="H37" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
@@ -2308,15 +2556,21 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" ht="31.5">
+      <c r="H38" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
@@ -2336,15 +2590,21 @@
       <c r="G39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" ht="31.5">
+      <c r="H39" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -2364,15 +2624,21 @@
       <c r="G40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" ht="31.5">
+      <c r="H40" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>104</v>
       </c>
@@ -2392,15 +2658,21 @@
         <v>89</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" ht="31.5">
+      <c r="H41" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>104</v>
       </c>
@@ -2420,15 +2692,21 @@
         <v>89</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" ht="31.5">
+      <c r="H42" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>104</v>
       </c>
@@ -2448,15 +2726,21 @@
         <v>89</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" ht="31.5">
+      <c r="H43" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>111</v>
       </c>
@@ -2474,15 +2758,21 @@
       <c r="G44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" ht="31.5">
+      <c r="H44" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>111</v>
       </c>
@@ -2500,15 +2790,21 @@
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:10" ht="47.25">
+      <c r="H45" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>117</v>
       </c>
@@ -2528,15 +2824,21 @@
         <v>52</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" ht="94.5">
+      <c r="H46" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>117</v>
       </c>
@@ -2558,15 +2860,21 @@
       <c r="G47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J47" s="1"/>
-    </row>
-    <row r="48" spans="1:10" ht="94.5">
+      <c r="H47" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>117</v>
       </c>
@@ -2588,15 +2896,21 @@
       <c r="G48" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" ht="47.25">
+      <c r="H48" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>117</v>
       </c>
@@ -2616,15 +2930,21 @@
         <v>89</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" ht="141.75">
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>126</v>
       </c>
@@ -2644,15 +2964,21 @@
       <c r="G50" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H50" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>126</v>
       </c>
@@ -2674,15 +3000,21 @@
       <c r="G51" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" ht="31.5">
+      <c r="H51" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>126</v>
       </c>
@@ -2702,15 +3034,21 @@
         <v>135</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52" s="1"/>
-    </row>
-    <row r="53" spans="1:10" ht="31.5">
+      <c r="H52" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>126</v>
       </c>
@@ -2730,15 +3068,21 @@
         <v>89</v>
       </c>
       <c r="G53" s="1"/>
-      <c r="H53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" ht="31.5">
+      <c r="H53" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>126</v>
       </c>
@@ -2758,15 +3102,21 @@
         <v>89</v>
       </c>
       <c r="G54" s="1"/>
-      <c r="H54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" ht="31.5">
+      <c r="H54" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>126</v>
       </c>
@@ -2786,15 +3136,21 @@
         <v>52</v>
       </c>
       <c r="G55" s="1"/>
-      <c r="H55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J55" s="1"/>
-    </row>
-    <row r="56" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H55" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>126</v>
       </c>
@@ -2816,15 +3172,21 @@
       <c r="G56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" ht="31.5">
+      <c r="H56" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L56" s="1"/>
+    </row>
+    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>126</v>
       </c>
@@ -2844,15 +3206,21 @@
         <v>52</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" s="1"/>
-    </row>
-    <row r="58" spans="1:10" ht="31.5">
+      <c r="H57" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>126</v>
       </c>
@@ -2872,15 +3240,21 @@
         <v>52</v>
       </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="1:10" ht="110.25">
+      <c r="H58" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>126</v>
       </c>
@@ -2902,22 +3276,28 @@
       <c r="G59" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H59" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" s="1"/>
+    </row>
+    <row r="60" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>154</v>
       </c>
       <c r="D60" s="7" t="s">
@@ -2928,22 +3308,28 @@
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="4" t="s">
+      <c r="H60" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J60" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J60" s="1"/>
-    </row>
-    <row r="61" spans="1:10" ht="31.5">
+      <c r="L60" s="1"/>
+    </row>
+    <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D61" s="4"/>
@@ -2952,15 +3338,21 @@
         <v>89</v>
       </c>
       <c r="G61" s="1"/>
-      <c r="H61" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J61" s="1"/>
-    </row>
-    <row r="62" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H61" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>155</v>
       </c>
@@ -2978,15 +3370,21 @@
       <c r="G62" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H62" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H62" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>155</v>
       </c>
@@ -3002,15 +3400,21 @@
         <v>164</v>
       </c>
       <c r="G63" s="1"/>
-      <c r="H63" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J63" s="1"/>
-    </row>
-    <row r="64" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H63" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>155</v>
       </c>
@@ -3024,15 +3428,21 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="1"/>
-      <c r="H64" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H64" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>155</v>
       </c>
@@ -3046,15 +3456,21 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J65" s="1"/>
-    </row>
-    <row r="66" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H65" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L65" s="1"/>
+    </row>
+    <row r="66" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>155</v>
       </c>
@@ -3070,15 +3486,21 @@
         <v>27</v>
       </c>
       <c r="G66" s="1"/>
-      <c r="H66" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I66" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J66" s="1"/>
-    </row>
-    <row r="67" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H66" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L66" s="1"/>
+    </row>
+    <row r="67" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>155</v>
       </c>
@@ -3096,15 +3518,21 @@
       <c r="G67" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H67" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I67" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J67" s="1"/>
-    </row>
-    <row r="68" spans="1:10" ht="32.25" customHeight="1">
+      <c r="H67" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" s="1"/>
+    </row>
+    <row r="68" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>155</v>
       </c>
@@ -3120,15 +3548,21 @@
         <v>27</v>
       </c>
       <c r="G68" s="1"/>
-      <c r="H68" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J68" s="1"/>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" customHeight="1">
+      <c r="H68" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L68" s="1"/>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>155</v>
       </c>
@@ -3144,15 +3578,21 @@
       <c r="G69" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H69" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="1:10" ht="31.5">
+      <c r="H69" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" s="1"/>
+    </row>
+    <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>155</v>
       </c>
@@ -3166,15 +3606,21 @@
       <c r="E70" s="6"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="4" t="s">
+      <c r="H70" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="I70" s="4" t="s">
+      <c r="K70" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" ht="47.25">
+      <c r="L70" s="1"/>
+    </row>
+    <row r="71" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>181</v>
       </c>
@@ -3194,15 +3640,21 @@
         <v>184</v>
       </c>
       <c r="G71" s="1"/>
-      <c r="H71" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="1:10" ht="47.25">
+      <c r="H71" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" s="1"/>
+    </row>
+    <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>181</v>
       </c>
@@ -3224,15 +3676,21 @@
       <c r="G72" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H72" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10" ht="47.25">
+      <c r="H72" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L72" s="1"/>
+    </row>
+    <row r="73" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>181</v>
       </c>
@@ -3252,15 +3710,21 @@
         <v>27</v>
       </c>
       <c r="G73" s="1"/>
-      <c r="H73" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" ht="47.25">
+      <c r="H73" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L73" s="1"/>
+    </row>
+    <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>181</v>
       </c>
@@ -3280,19 +3744,25 @@
         <v>192</v>
       </c>
       <c r="G74" s="1"/>
-      <c r="H74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J74" s="1"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="11" t="s">
+      <c r="H74" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I74" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L74" s="1"/>
+    </row>
+    <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="10" t="s">
         <v>219</v>
       </c>
       <c r="C75" s="6" t="s">
@@ -3304,15 +3774,21 @@
       <c r="E75" t="s">
         <v>222</v>
       </c>
-      <c r="H75" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I75" s="4" t="s">
+      <c r="H75" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K75" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H117" xr:uid="{F7C77282-C0D9-FE44-835B-2F72376F6C5B}"/>
+  <autoFilter ref="J1:J117" xr:uid="{F7C77282-C0D9-FE44-835B-2F72376F6C5B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Change formatting of "Entries" for factor variables.
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzprante/GitHub/MORPEP/META CMP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58FBF8B-6395-B441-9C58-DC78FE6E25B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED2E915-88EF-6A49-821C-B66C22BAA702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{4AE10940-A047-2F4D-80AE-0938BE2B299E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{4AE10940-A047-2F4D-80AE-0938BE2B299E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,9 +649,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>"fp","me"</t>
-  </si>
-  <si>
     <t>numeric</t>
   </si>
   <si>
@@ -659,9 +656,6 @@
   </si>
   <si>
     <t>true; false</t>
-  </si>
-  <si>
-    <t>"3_month_repo"</t>
   </si>
   <si>
     <r>
@@ -682,16 +676,10 @@
     <t xml:space="preserve">Shock size in basis points e.g., 100 = 1pp. How to deal with 1% shock? </t>
   </si>
   <si>
-    <t>"68"; "90"; "95"; "1_SE"; "2_SE"; "80"</t>
-  </si>
-  <si>
     <t>factor</t>
   </si>
   <si>
     <t>1 if outcome variable is of main research interest for the paper</t>
-  </si>
-  <si>
-    <t>"gdp"; "emp"; "inflation"; "other"</t>
   </si>
   <si>
     <t>xxx</t>
@@ -768,17 +756,11 @@
 for yearly data: "%Y"</t>
   </si>
   <si>
-    <t>"lev_ngdp";  "logdiff_rgap"; "growth_rIP"; "logdiff_une"; "lev_emp"; "growth_CPI"</t>
-  </si>
-  <si>
     <t>for bp shock: "xxxbp"
 for % shock:
 "xxx%"
 for SE shock (if no information on SE size):
 "xxxSE"</t>
-  </si>
-  <si>
-    <t>"ardl"; "ecm"</t>
   </si>
   <si>
     <r>
@@ -844,6 +826,24 @@
   </si>
   <si>
     <t>public_database</t>
+  </si>
+  <si>
+    <t>3_month_repo</t>
+  </si>
+  <si>
+    <t>fp me</t>
+  </si>
+  <si>
+    <t>68  90  95  1_SE  2_SE  80</t>
+  </si>
+  <si>
+    <t>gdp  emp  inflation  other</t>
+  </si>
+  <si>
+    <t>ardl  ecm</t>
+  </si>
+  <si>
+    <t>lev_ngdp  logdiff_rgap  growth_rIP  logdiff_une  lev_emp  growth_CPI</t>
   </si>
 </sst>
 </file>
@@ -943,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -974,9 +974,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1298,7 +1295,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I76" sqref="I76"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1304,7 @@
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="87.1640625" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="68.33203125" customWidth="1"/>
     <col min="6" max="9" width="40.6640625" customWidth="1"/>
     <col min="10" max="11" width="17.5" customWidth="1"/>
   </cols>
@@ -1335,10 +1332,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>5</v>
@@ -1366,11 +1363,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>228</v>
+      <c r="H2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="4" t="s">
@@ -1389,18 +1386,18 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>229</v>
+      <c r="H3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
@@ -1419,18 +1416,18 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>229</v>
+      <c r="H4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -1454,11 +1451,11 @@
       <c r="E5" s="6"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>229</v>
+      <c r="H5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -1482,11 +1479,11 @@
       <c r="E6" s="1"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>229</v>
+      <c r="H6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -1502,21 +1499,21 @@
         <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>230</v>
+      <c r="H7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>11</v>
@@ -1534,21 +1531,21 @@
         <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>230</v>
+      <c r="H8" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>11</v>
@@ -1566,21 +1563,21 @@
         <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>230</v>
+      <c r="H9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>11</v>
@@ -1598,23 +1595,23 @@
         <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>230</v>
+      <c r="H10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>11</v>
@@ -1632,23 +1629,23 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>230</v>
+      <c r="H11" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>11</v>
@@ -1666,21 +1663,21 @@
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>230</v>
+      <c r="H12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>11</v>
@@ -1698,21 +1695,21 @@
         <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>230</v>
+      <c r="H13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>11</v>
@@ -1730,21 +1727,21 @@
         <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>230</v>
+      <c r="H14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>11</v>
@@ -1765,20 +1762,20 @@
         <v>34</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>230</v>
+      <c r="H15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>11</v>
@@ -1799,10 +1796,10 @@
         <v>38</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
@@ -1810,11 +1807,11 @@
       <c r="G16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>230</v>
+      <c r="H16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>11</v>
@@ -1835,20 +1832,20 @@
         <v>42</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>230</v>
+      <c r="H17" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>11</v>
@@ -1869,10 +1866,10 @@
         <v>44</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>31</v>
@@ -1880,11 +1877,11 @@
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>230</v>
+      <c r="H18" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>11</v>
@@ -1905,10 +1902,10 @@
         <v>47</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1916,11 +1913,11 @@
       <c r="G19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>230</v>
+      <c r="H19" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>11</v>
@@ -1941,10 +1938,10 @@
         <v>51</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>52</v>
@@ -1952,11 +1949,11 @@
       <c r="G20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>230</v>
+      <c r="H20" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>11</v>
@@ -1977,10 +1974,10 @@
         <v>55</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>48</v>
@@ -1988,11 +1985,11 @@
       <c r="G21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>230</v>
+      <c r="H21" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>11</v>
@@ -2013,10 +2010,10 @@
         <v>58</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>59</v>
@@ -2024,11 +2021,11 @@
       <c r="G22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>230</v>
+      <c r="H22" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>11</v>
@@ -2049,20 +2046,20 @@
         <v>62</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>230</v>
+      <c r="H23" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>11</v>
@@ -2083,20 +2080,20 @@
         <v>65</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>230</v>
+      <c r="H24" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>11</v>
@@ -2117,20 +2114,20 @@
         <v>67</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>230</v>
+      <c r="H25" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>11</v>
@@ -2151,20 +2148,20 @@
         <v>70</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>230</v>
+      <c r="H26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>11</v>
@@ -2185,20 +2182,20 @@
         <v>72</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>230</v>
+      <c r="H27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>11</v>
@@ -2219,20 +2216,20 @@
         <v>74</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>230</v>
+      <c r="H28" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>11</v>
@@ -2250,21 +2247,21 @@
         <v>75</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>230</v>
+      <c r="H29" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>11</v>
@@ -2285,20 +2282,20 @@
         <v>77</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="H30" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>230</v>
+      <c r="H30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>11</v>
@@ -2319,20 +2316,20 @@
         <v>80</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>230</v>
+      <c r="H31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>11</v>
@@ -2353,18 +2350,18 @@
         <v>82</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>230</v>
+      <c r="H32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>83</v>
@@ -2385,20 +2382,20 @@
         <v>85</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>230</v>
+      <c r="H33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>11</v>
@@ -2419,18 +2416,18 @@
         <v>87</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>230</v>
+      <c r="H34" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>11</v>
@@ -2451,20 +2448,20 @@
         <v>91</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>230</v>
+      <c r="H35" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>11</v>
@@ -2485,18 +2482,18 @@
         <v>94</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>230</v>
+      <c r="H36" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>11</v>
@@ -2517,18 +2514,18 @@
         <v>96</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>230</v>
+      <c r="H37" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>11</v>
@@ -2549,18 +2546,18 @@
         <v>98</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>230</v>
+      <c r="H38" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>11</v>
@@ -2581,20 +2578,20 @@
         <v>100</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>230</v>
+      <c r="H39" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>11</v>
@@ -2615,20 +2612,20 @@
         <v>103</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>230</v>
+      <c r="H40" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>11</v>
@@ -2649,20 +2646,20 @@
         <v>106</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>230</v>
+      <c r="H41" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>11</v>
@@ -2683,20 +2680,20 @@
         <v>108</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>230</v>
+      <c r="H42" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>11</v>
@@ -2717,20 +2714,20 @@
         <v>110</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>230</v>
+      <c r="H43" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>11</v>
@@ -2758,11 +2755,11 @@
       <c r="G44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H44" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>230</v>
+      <c r="H44" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>11</v>
@@ -2783,18 +2780,18 @@
         <v>116</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>230</v>
+      <c r="H45" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>11</v>
@@ -2815,20 +2812,20 @@
         <v>119</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>230</v>
+      <c r="H46" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>11</v>
@@ -2846,13 +2843,13 @@
         <v>120</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>195</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>52</v>
@@ -2860,11 +2857,11 @@
       <c r="G47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H47" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>230</v>
+      <c r="H47" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>11</v>
@@ -2882,13 +2879,13 @@
         <v>122</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>195</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>52</v>
@@ -2896,11 +2893,11 @@
       <c r="G48" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H48" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>230</v>
+      <c r="H48" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>11</v>
@@ -2921,20 +2918,20 @@
         <v>124</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="11" t="s">
+      <c r="H49" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>125</v>
@@ -2955,20 +2952,20 @@
         <v>128</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H50" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>230</v>
+      <c r="H50" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>11</v>
@@ -2989,10 +2986,10 @@
         <v>131</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>89</v>
@@ -3000,11 +2997,11 @@
       <c r="G51" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H51" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I51" s="11" t="s">
-        <v>230</v>
+      <c r="H51" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>11</v>
@@ -3025,20 +3022,20 @@
         <v>134</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>135</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>230</v>
+      <c r="H52" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>11</v>
@@ -3059,20 +3056,20 @@
         <v>137</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G53" s="1"/>
-      <c r="H53" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I53" s="11" t="s">
-        <v>230</v>
+      <c r="H53" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>11</v>
@@ -3093,20 +3090,20 @@
         <v>139</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G54" s="1"/>
-      <c r="H54" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>230</v>
+      <c r="H54" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>11</v>
@@ -3127,20 +3124,20 @@
         <v>141</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G55" s="1"/>
-      <c r="H55" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>230</v>
+      <c r="H55" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>11</v>
@@ -3161,10 +3158,10 @@
         <v>143</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>31</v>
@@ -3172,11 +3169,11 @@
       <c r="G56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H56" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>230</v>
+      <c r="H56" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>11</v>
@@ -3197,20 +3194,20 @@
         <v>146</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>230</v>
+      <c r="H57" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>11</v>
@@ -3231,20 +3228,20 @@
         <v>148</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>230</v>
+      <c r="H58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>11</v>
@@ -3265,10 +3262,10 @@
         <v>150</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>52</v>
@@ -3276,11 +3273,11 @@
       <c r="G59" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H59" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I59" s="11" t="s">
-        <v>230</v>
+      <c r="H59" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>11</v>
@@ -3301,18 +3298,18 @@
         <v>154</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I60" s="11" t="s">
-        <v>230</v>
+      <c r="H60" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>83</v>
@@ -3338,11 +3335,11 @@
         <v>89</v>
       </c>
       <c r="G61" s="1"/>
-      <c r="H61" s="11" t="s">
+      <c r="H61" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>11</v>
@@ -3370,11 +3367,11 @@
       <c r="G62" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H62" s="11" t="s">
+      <c r="H62" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>11</v>
@@ -3400,11 +3397,11 @@
         <v>164</v>
       </c>
       <c r="G63" s="1"/>
-      <c r="H63" s="11" t="s">
+      <c r="H63" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I63" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>11</v>
@@ -3428,11 +3425,11 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="1"/>
-      <c r="H64" s="11" t="s">
+      <c r="H64" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>11</v>
@@ -3456,11 +3453,11 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="11" t="s">
+      <c r="H65" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I65" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>11</v>
@@ -3486,11 +3483,11 @@
         <v>27</v>
       </c>
       <c r="G66" s="1"/>
-      <c r="H66" s="11" t="s">
+      <c r="H66" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I66" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>11</v>
@@ -3518,11 +3515,11 @@
       <c r="G67" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H67" s="11" t="s">
+      <c r="H67" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I67" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>11</v>
@@ -3548,11 +3545,11 @@
         <v>27</v>
       </c>
       <c r="G68" s="1"/>
-      <c r="H68" s="11" t="s">
+      <c r="H68" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>11</v>
@@ -3578,11 +3575,11 @@
       <c r="G69" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H69" s="11" t="s">
+      <c r="H69" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I69" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>11</v>
@@ -3606,11 +3603,11 @@
       <c r="E70" s="6"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="11" t="s">
+      <c r="H70" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>125</v>
@@ -3631,20 +3628,20 @@
         <v>183</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>184</v>
       </c>
       <c r="G71" s="1"/>
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>11</v>
@@ -3665,10 +3662,10 @@
         <v>186</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>184</v>
@@ -3676,11 +3673,11 @@
       <c r="G72" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H72" s="11" t="s">
+      <c r="H72" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>11</v>
@@ -3701,20 +3698,20 @@
         <v>189</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>27</v>
       </c>
       <c r="G73" s="1"/>
-      <c r="H73" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I73" s="11" t="s">
-        <v>230</v>
+      <c r="H73" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>11</v>
@@ -3735,20 +3732,20 @@
         <v>191</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>192</v>
       </c>
       <c r="G74" s="1"/>
-      <c r="H74" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="I74" s="11" t="s">
-        <v>229</v>
+      <c r="H74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>11</v>
@@ -3760,25 +3757,25 @@
     </row>
     <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C75" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E75" t="s">
+        <v>216</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E75" t="s">
-        <v>222</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="I75" s="11" t="s">
-        <v>229</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Update of codes for `dep` #10
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzprante/GitHub/MORPEP/META CMP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED2E915-88EF-6A49-821C-B66C22BAA702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8E2CE8-93AC-FD46-84FF-BA27F6A75AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{4AE10940-A047-2F4D-80AE-0938BE2B299E}"/>
   </bookViews>
@@ -843,7 +843,7 @@
     <t>ardl  ecm</t>
   </si>
   <si>
-    <t>lev_ngdp  logdiff_rgap  growth_rIP  logdiff_une  lev_emp  growth_CPI</t>
+    <t>lev_rgdp log_rgdp logdiff_rgdp gr_rgdp lev_ngdp log_ngdp logdiff_ngdp logdiff_ngdp growth_rIP logdiff_rgap lev_emp logdiff_une growth_CPI</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>117</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
Correction in codes for `dep` #10
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzprante/GitHub/MORPEP/META CMP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8E2CE8-93AC-FD46-84FF-BA27F6A75AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A2B8C-74C1-8740-B2E2-2B41B4853C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{4AE10940-A047-2F4D-80AE-0938BE2B299E}"/>
   </bookViews>
@@ -843,7 +843,7 @@
     <t>ardl  ecm</t>
   </si>
   <si>
-    <t>lev_rgdp log_rgdp logdiff_rgdp gr_rgdp lev_ngdp log_ngdp logdiff_ngdp logdiff_ngdp growth_rIP logdiff_rgap lev_emp logdiff_une growth_CPI</t>
+    <t>lev_rgdp log_rgdp logdiff_rgdp gr_rgdp lev_ngdp log_ngdp logdiff_ngdp logdiff_ngdp growth_rip logdiff_rgap lev_emp logdiff_une growth_cpi</t>
   </si>
 </sst>
 </file>

</xml_diff>